<commit_message>
Drafted model for the toursim goal. mean score of resident sentiment, nearshore water protection, and visitor generated gdp.
</commit_message>
<xml_diff>
--- a/prep/TR/sentiment.xlsx
+++ b/prep/TR/sentiment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="24915" windowHeight="6720"/>
+    <workbookView minimized="1" xWindow="-4005" yWindow="2115" windowWidth="24915" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,14 +446,14 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>

</xml_diff>